<commit_message>
Modify - Team Column
Modified the algorithm to add the team name to the excel file.
</commit_message>
<xml_diff>
--- a/output_stuff/single_event_results.xlsx
+++ b/output_stuff/single_event_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,25 +461,30 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Team Name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Order</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Leg</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Cumulative</t>
         </is>
@@ -511,23 +516,28 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Caribe, Guilherme JR</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>19.28</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>40.57</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>40.57</t>
         </is>
@@ -559,23 +569,28 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Taylor, Lamar 5Y</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>2</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>19.11</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>41.02</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>1:21.59</t>
         </is>
@@ -607,23 +622,28 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Blackman, Nikoli SO</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>3</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>19.36</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>41.35</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>2:02.94</t>
         </is>
@@ -655,23 +675,28 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Crooks, Jordan SR</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>4</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>18.35</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>39.36</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>2:42.30</t>
         </is>
@@ -703,23 +728,28 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>ASU</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Kharun, Ilya SO</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>19.65</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>41.24</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>41.24</t>
         </is>
@@ -751,23 +781,28 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>ASU</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>Sammon, Patrick SR</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>2</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>18.98</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>40.55</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>1:21.79</t>
         </is>
@@ -799,23 +834,28 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>ASU</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Palmer, Tommy JR</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>3</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>19.20</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>41.50</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>2:03.29</t>
         </is>
@@ -847,23 +887,28 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>ASU</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Kulow, Jonny JR</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>4</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>18.79</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>39.93</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>2:43.22</t>
         </is>
@@ -895,23 +940,28 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Liendo, Josh JR</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>19.11</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>40.42</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>40.42</t>
         </is>
@@ -943,23 +993,28 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Smith, Julian SR</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>2</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>19.21</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>40.96</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>1:21.38</t>
         </is>
@@ -991,23 +1046,28 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Painter, Alexander FR</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>3</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>19.39</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>41.18</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>2:02.56</t>
         </is>
@@ -1039,23 +1099,28 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>Buff, Scott SO</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>4</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>19.48</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>41.46</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>2:44.02</t>
         </is>
@@ -1087,23 +1152,28 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Alexy, Jack SR</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>19.36</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>40.55</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>40.55</t>
         </is>
@@ -1135,23 +1205,28 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Seeliger, Bjorn 5Y</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>2</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>19.36</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>41.29</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>1:21.84</t>
         </is>
@@ -1183,23 +1258,28 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>Jensen, Matthew 5Y</t>
         </is>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>3</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>19.48</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>41.30</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>2:03.14</t>
         </is>
@@ -1231,23 +1311,28 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Lasco, Destin 5Y</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>4</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>19.62</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>41.45</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>2:44.59</t>
         </is>
@@ -1279,23 +1364,28 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>McDonald, Owen JR</t>
         </is>
       </c>
-      <c r="G18" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>19.93</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>41.41</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>41.41</t>
         </is>
@@ -1327,23 +1417,28 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>King, Matthew JR</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>2</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>19.14</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>40.78</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>1:22.19</t>
         </is>
@@ -1375,23 +1470,28 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>Smiley, Dylan SO</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>3</v>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>19.87</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>41.77</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>2:03.96</t>
         </is>
@@ -1423,23 +1523,28 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>Miroslaw, Rafael SR</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>4</v>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>19.17</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>41.12</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>2:45.08</t>
         </is>
@@ -1471,23 +1576,28 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>NC State</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>McCarty, Quintin SO</t>
         </is>
       </c>
-      <c r="G22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" t="inlineStr">
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>19.61</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>41.58</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>41.58</t>
         </is>
@@ -1519,23 +1629,28 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>NC State</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>Fox, Jerry SO</t>
         </is>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>2</v>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>19.23</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>41.05</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>1:22.63</t>
         </is>
@@ -1567,23 +1682,28 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>NC State</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Miller, Luke 5Y</t>
         </is>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>3</v>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>19.55</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>41.33</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>2:03.96</t>
         </is>
@@ -1615,23 +1735,28 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>NC State</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>Hoover, Sam SR</t>
         </is>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>4</v>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>19.49</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>41.13</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>2:45.09</t>
         </is>
@@ -1663,23 +1788,28 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Guiliano, Chris SR</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" t="inlineStr">
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>19.48</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>40.84</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>40.84</t>
         </is>
@@ -1711,23 +1841,28 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>Kos, Hubert JR</t>
         </is>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>2</v>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>19.72</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>41.35</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>1:22.19</t>
         </is>
@@ -1759,23 +1894,28 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Maurer, Rex SO</t>
         </is>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>3</v>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>19.91</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>42.04</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>2:04.23</t>
         </is>
@@ -1807,23 +1947,28 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>Hobson, Luke SR</t>
         </is>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>4</v>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>19.46</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>40.89</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>2:45.12</t>
         </is>
@@ -1855,23 +2000,28 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>VT</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>Ramadan, Youssef 5Y</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" t="inlineStr">
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>19.86</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>41.44</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>41.44</t>
         </is>
@@ -1903,23 +2053,28 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t>VT</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>Whitfield, Brendan SO</t>
         </is>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>2</v>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>19.28</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="J31" t="inlineStr">
         <is>
           <t>41.04</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="K31" t="inlineStr">
         <is>
           <t>1:22.48</t>
         </is>
@@ -1951,23 +2106,28 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>VT</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>Coll Marti, Carles 5Y</t>
         </is>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>3</v>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>19.87</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>42.11</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t>2:04.59</t>
         </is>
@@ -1999,23 +2159,28 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>VT</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>Molla Yanes, Mario SR</t>
         </is>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>4</v>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>19.46</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>41.62</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="K33" t="inlineStr">
         <is>
           <t>2:46.21</t>
         </is>
@@ -2047,23 +2212,28 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>Wilson, Zarek SO</t>
         </is>
       </c>
-      <c r="G34" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" t="inlineStr">
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>20.26</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>42.32</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>42.32</t>
         </is>
@@ -2095,23 +2265,28 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>Hawke, Charlie SR</t>
         </is>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>2</v>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>19.36</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>41.09</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>1:23.41</t>
         </is>
@@ -2143,23 +2318,28 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>Alves, Kaique SR</t>
         </is>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>3</v>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>19.70</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="J36" t="inlineStr">
         <is>
           <t>41.62</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="K36" t="inlineStr">
         <is>
           <t>2:05.03</t>
         </is>
@@ -2191,23 +2371,28 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>Dragoja, Toni JR</t>
         </is>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>4</v>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>19.73</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>41.37</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>2:46.40</t>
         </is>
@@ -2239,23 +2424,28 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>Dupont Cabrera, Andres JR</t>
         </is>
       </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="inlineStr">
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="inlineStr">
         <is>
           <t>20.07</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="J38" t="inlineStr">
         <is>
           <t>41.94</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>41.94</t>
         </is>
@@ -2287,23 +2477,28 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>Minakov, Andrei SR</t>
         </is>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>2</v>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>19.29</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="J39" t="inlineStr">
         <is>
           <t>41.33</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="K39" t="inlineStr">
         <is>
           <t>1:23.27</t>
         </is>
@@ -2335,23 +2530,28 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>Gu, Rafael JR</t>
         </is>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>3</v>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>19.42</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="J40" t="inlineStr">
         <is>
           <t>41.69</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>2:04.96</t>
         </is>
@@ -2383,23 +2583,28 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>McFadden, Henry SO</t>
         </is>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>4</v>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>20.05</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t>42.07</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="K41" t="inlineStr">
         <is>
           <t>2:47.03</t>
         </is>
@@ -2431,23 +2636,28 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
           <t>Urlando, Gianluca 5Y</t>
         </is>
       </c>
-      <c r="G42" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" t="inlineStr">
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>19.80</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="J42" t="inlineStr">
         <is>
           <t>41.58</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="K42" t="inlineStr">
         <is>
           <t>41.58</t>
         </is>
@@ -2479,23 +2689,28 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>Magahey, Jake 5Y</t>
         </is>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>2</v>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>19.97</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="J43" t="inlineStr">
         <is>
           <t>42.07</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>1:23.65</t>
         </is>
@@ -2527,23 +2742,28 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>Koski, Tomas SO</t>
         </is>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>3</v>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>19.83</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="J44" t="inlineStr">
         <is>
           <t>41.60</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="K44" t="inlineStr">
         <is>
           <t>2:05.25</t>
         </is>
@@ -2575,23 +2795,28 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>Branzell, Reese SR</t>
         </is>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>4</v>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="I45" t="inlineStr">
         <is>
           <t>19.73</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
+      <c r="J45" t="inlineStr">
         <is>
           <t>41.90</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>2:47.15</t>
         </is>
@@ -2623,23 +2848,28 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>Lukminas, Tomas FR</t>
         </is>
       </c>
-      <c r="G46" t="n">
-        <v>1</v>
-      </c>
-      <c r="H46" t="inlineStr">
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>19.89</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="J46" t="inlineStr">
         <is>
           <t>41.95</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="K46" t="inlineStr">
         <is>
           <t>41.95</t>
         </is>
@@ -2671,23 +2901,28 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
           <t>Daleiden Ciuferalph JR</t>
         </is>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>2</v>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>19.57</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="J47" t="inlineStr">
         <is>
           <t>41.59</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="K47" t="inlineStr">
         <is>
           <t>1:23.54</t>
         </is>
@@ -2719,23 +2954,28 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
           <t>Nabor, Jadan SR</t>
         </is>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>3</v>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="I48" t="inlineStr">
         <is>
           <t>19.59</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>42.10</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="K48" t="inlineStr">
         <is>
           <t>2:05.64</t>
         </is>
@@ -2767,23 +3007,28 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
           <t>Ingram, Hunter 5Y</t>
         </is>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>4</v>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="I49" t="inlineStr">
         <is>
           <t>19.63</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>42.00</t>
         </is>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="K49" t="inlineStr">
         <is>
           <t>2:47.64</t>
         </is>
@@ -2815,23 +3060,28 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
+          <t>OSU</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
           <t>Navikonis, Tomas JR</t>
         </is>
       </c>
-      <c r="G50" t="n">
-        <v>1</v>
-      </c>
-      <c r="H50" t="inlineStr">
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="inlineStr">
         <is>
           <t>20.24</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
+      <c r="J50" t="inlineStr">
         <is>
           <t>41.96</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="K50" t="inlineStr">
         <is>
           <t>41.96</t>
         </is>
@@ -2863,23 +3113,28 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
+          <t>OSU</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
           <t>Baltes, Daniel SR</t>
         </is>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>2</v>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="I51" t="inlineStr">
         <is>
           <t>19.67</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
+      <c r="J51" t="inlineStr">
         <is>
           <t>41.52</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="K51" t="inlineStr">
         <is>
           <t>1:23.48</t>
         </is>
@@ -2911,23 +3166,28 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>OSU</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
           <t>McDonald, Mario 5Y</t>
         </is>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>3</v>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="I52" t="inlineStr">
         <is>
           <t>19.81</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="J52" t="inlineStr">
         <is>
           <t>42.14</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="K52" t="inlineStr">
         <is>
           <t>2:05.62</t>
         </is>
@@ -2959,23 +3219,28 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
+          <t>OSU</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
           <t>Jahn, Cornelius FR</t>
         </is>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>4</v>
       </c>
-      <c r="H53" t="inlineStr">
+      <c r="I53" t="inlineStr">
         <is>
           <t>20.13</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="J53" t="inlineStr">
         <is>
           <t>42.07</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="K53" t="inlineStr">
         <is>
           <t>2:47.69</t>
         </is>
@@ -3007,23 +3272,28 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
+          <t>TAMU</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
           <t>Foote, Connor JR</t>
         </is>
       </c>
-      <c r="G54" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" t="inlineStr">
+      <c r="H54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" t="inlineStr">
         <is>
           <t>19.52</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr">
+      <c r="J54" t="inlineStr">
         <is>
           <t>41.58</t>
         </is>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="K54" t="inlineStr">
         <is>
           <t>41.58</t>
         </is>
@@ -3055,23 +3325,28 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
+          <t>TAMU</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
           <t>Scholl, Benjamin SO</t>
         </is>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>2</v>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="I55" t="inlineStr">
         <is>
           <t>19.52</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="J55" t="inlineStr">
         <is>
           <t>41.63</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="K55" t="inlineStr">
         <is>
           <t>1:23.21</t>
         </is>
@@ -3103,23 +3378,28 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
+          <t>TAMU</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
           <t>Reno, Seth JR</t>
         </is>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>3</v>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="I56" t="inlineStr">
         <is>
           <t>19.62</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr">
+      <c r="J56" t="inlineStr">
         <is>
           <t>42.51</t>
         </is>
       </c>
-      <c r="J56" t="inlineStr">
+      <c r="K56" t="inlineStr">
         <is>
           <t>2:05.72</t>
         </is>
@@ -3151,23 +3431,28 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
+          <t>TAMU</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
           <t>Wimberly, Jacob FR</t>
         </is>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>4</v>
       </c>
-      <c r="H57" t="inlineStr">
+      <c r="I57" t="inlineStr">
         <is>
           <t>19.64</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr">
+      <c r="J57" t="inlineStr">
         <is>
           <t>42.36</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="K57" t="inlineStr">
         <is>
           <t>2:48.08</t>
         </is>
@@ -3199,23 +3484,28 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
           <t>Brooks, Guy JR</t>
         </is>
       </c>
-      <c r="G58" t="n">
-        <v>1</v>
-      </c>
-      <c r="H58" t="inlineStr">
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" t="inlineStr">
         <is>
           <t>20.07</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr">
+      <c r="J58" t="inlineStr">
         <is>
           <t>42.20</t>
         </is>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="K58" t="inlineStr">
         <is>
           <t>42.20</t>
         </is>
@@ -3247,23 +3537,28 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
           <t>Lowe, Dalton 5Y</t>
         </is>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>2</v>
       </c>
-      <c r="H59" t="inlineStr">
+      <c r="I59" t="inlineStr">
         <is>
           <t>19.38</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr">
+      <c r="J59" t="inlineStr">
         <is>
           <t>42.08</t>
         </is>
       </c>
-      <c r="J59" t="inlineStr">
+      <c r="K59" t="inlineStr">
         <is>
           <t>1:24.28</t>
         </is>
@@ -3295,23 +3590,28 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
           <t>Sartori, Murilo SR</t>
         </is>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>3</v>
       </c>
-      <c r="H60" t="inlineStr">
+      <c r="I60" t="inlineStr">
         <is>
           <t>19.68</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr">
+      <c r="J60" t="inlineStr">
         <is>
           <t>41.77</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
+      <c r="K60" t="inlineStr">
         <is>
           <t>2:06.05</t>
         </is>
@@ -3343,23 +3643,28 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
           <t>Graham, Rian FR</t>
         </is>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>4</v>
       </c>
-      <c r="H61" t="inlineStr">
+      <c r="I61" t="inlineStr">
         <is>
           <t>19.58</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr">
+      <c r="J61" t="inlineStr">
         <is>
           <t>42.15</t>
         </is>
       </c>
-      <c r="J61" t="inlineStr">
+      <c r="K61" t="inlineStr">
         <is>
           <t>2:48.20</t>
         </is>
@@ -3391,23 +3696,28 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
           <t>Aikins, Jack JR</t>
         </is>
       </c>
-      <c r="G62" t="n">
-        <v>1</v>
-      </c>
-      <c r="H62" t="inlineStr">
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="inlineStr">
         <is>
           <t>20.37</t>
         </is>
       </c>
-      <c r="I62" t="inlineStr">
+      <c r="J62" t="inlineStr">
         <is>
           <t>42.70</t>
         </is>
       </c>
-      <c r="J62" t="inlineStr">
+      <c r="K62" t="inlineStr">
         <is>
           <t>42.70</t>
         </is>
@@ -3439,23 +3749,28 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
           <t>Boyle, Conor SR</t>
         </is>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>2</v>
       </c>
-      <c r="H63" t="inlineStr">
+      <c r="I63" t="inlineStr">
         <is>
           <t>19.33</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr">
+      <c r="J63" t="inlineStr">
         <is>
           <t>41.47</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="K63" t="inlineStr">
         <is>
           <t>1:24.17</t>
         </is>
@@ -3487,23 +3802,28 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
           <t>Nicholas, Spencer FR</t>
         </is>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>3</v>
       </c>
-      <c r="H64" t="inlineStr">
+      <c r="I64" t="inlineStr">
         <is>
           <t>20.26</t>
         </is>
       </c>
-      <c r="I64" t="inlineStr">
+      <c r="J64" t="inlineStr">
         <is>
           <t>42.43</t>
         </is>
       </c>
-      <c r="J64" t="inlineStr">
+      <c r="K64" t="inlineStr">
         <is>
           <t>2:06.60</t>
         </is>
@@ -3535,23 +3855,28 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>Sergile, Sebastien JR</t>
         </is>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>4</v>
       </c>
-      <c r="H65" t="inlineStr">
+      <c r="I65" t="inlineStr">
         <is>
           <t>20.10</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr">
+      <c r="J65" t="inlineStr">
         <is>
           <t>41.96</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="K65" t="inlineStr">
         <is>
           <t>2:48.56</t>
         </is>
@@ -3583,23 +3908,28 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
+          <t>FSU</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
           <t>Arkhangelskiy, Michel FR</t>
         </is>
       </c>
-      <c r="G66" t="n">
-        <v>1</v>
-      </c>
-      <c r="H66" t="inlineStr">
+      <c r="H66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>19.88</t>
         </is>
       </c>
-      <c r="I66" t="inlineStr">
+      <c r="J66" t="inlineStr">
         <is>
           <t>41.84</t>
         </is>
       </c>
-      <c r="J66" t="inlineStr">
+      <c r="K66" t="inlineStr">
         <is>
           <t>41.84</t>
         </is>
@@ -3631,23 +3961,28 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
+          <t>FSU</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
           <t>Herbet, Mason 5Y</t>
         </is>
       </c>
-      <c r="G67" t="n">
+      <c r="H67" t="n">
         <v>2</v>
       </c>
-      <c r="H67" t="inlineStr">
+      <c r="I67" t="inlineStr">
         <is>
           <t>19.84</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr">
+      <c r="J67" t="inlineStr">
         <is>
           <t>42.17</t>
         </is>
       </c>
-      <c r="J67" t="inlineStr">
+      <c r="K67" t="inlineStr">
         <is>
           <t>1:24.01</t>
         </is>
@@ -3679,23 +4014,28 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
+          <t>FSU</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
           <t>Wilson, Max JR</t>
         </is>
       </c>
-      <c r="G68" t="n">
+      <c r="H68" t="n">
         <v>3</v>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="I68" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="J68" t="inlineStr">
         <is>
           <t>42.24</t>
         </is>
       </c>
-      <c r="J68" t="inlineStr">
+      <c r="K68" t="inlineStr">
         <is>
           <t>2:06.25</t>
         </is>
@@ -3727,23 +4067,28 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
+          <t>FSU</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
           <t>Yanchev, Yordan 5Y</t>
         </is>
       </c>
-      <c r="G69" t="n">
+      <c r="H69" t="n">
         <v>4</v>
       </c>
-      <c r="H69" t="inlineStr">
+      <c r="I69" t="inlineStr">
         <is>
           <t>20.10</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr">
+      <c r="J69" t="inlineStr">
         <is>
           <t>42.75</t>
         </is>
       </c>
-      <c r="J69" t="inlineStr">
+      <c r="K69" t="inlineStr">
         <is>
           <t>2:49.00</t>
         </is>
@@ -3775,23 +4120,28 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
           <t>Wilkening, Jack JR</t>
         </is>
       </c>
-      <c r="G70" t="n">
-        <v>1</v>
-      </c>
-      <c r="H70" t="inlineStr">
+      <c r="H70" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" t="inlineStr">
         <is>
           <t>20.26</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr">
+      <c r="J70" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
       </c>
-      <c r="J70" t="inlineStr">
+      <c r="K70" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
@@ -3823,23 +4173,28 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
           <t>Szabados, Bence 5Y</t>
         </is>
       </c>
-      <c r="G71" t="n">
+      <c r="H71" t="n">
         <v>2</v>
       </c>
-      <c r="H71" t="inlineStr">
+      <c r="I71" t="inlineStr">
         <is>
           <t>19.67</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr">
+      <c r="J71" t="inlineStr">
         <is>
           <t>42.34</t>
         </is>
       </c>
-      <c r="J71" t="inlineStr">
+      <c r="K71" t="inlineStr">
         <is>
           <t>1:24.74</t>
         </is>
@@ -3871,23 +4226,28 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
           <t>Geer, Colin SO</t>
         </is>
       </c>
-      <c r="G72" t="n">
+      <c r="H72" t="n">
         <v>3</v>
       </c>
-      <c r="H72" t="inlineStr">
+      <c r="I72" t="inlineStr">
         <is>
           <t>20.24</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr">
+      <c r="J72" t="inlineStr">
         <is>
           <t>42.54</t>
         </is>
       </c>
-      <c r="J72" t="inlineStr">
+      <c r="K72" t="inlineStr">
         <is>
           <t>2:07.28</t>
         </is>
@@ -3919,23 +4279,28 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
           <t>Groumi, Gal SR</t>
         </is>
       </c>
-      <c r="G73" t="n">
+      <c r="H73" t="n">
         <v>4</v>
       </c>
-      <c r="H73" t="inlineStr">
+      <c r="I73" t="inlineStr">
         <is>
           <t>19.80</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr">
+      <c r="J73" t="inlineStr">
         <is>
           <t>41.81</t>
         </is>
       </c>
-      <c r="J73" t="inlineStr">
+      <c r="K73" t="inlineStr">
         <is>
           <t>2:49.09</t>
         </is>
@@ -3967,23 +4332,28 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
           <t>Morris, Christopher SR</t>
         </is>
       </c>
-      <c r="G74" t="n">
-        <v>1</v>
-      </c>
-      <c r="H74" t="inlineStr">
+      <c r="H74" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" t="inlineStr">
         <is>
           <t>20.27</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="J74" t="inlineStr">
         <is>
           <t>42.28</t>
         </is>
       </c>
-      <c r="J74" t="inlineStr">
+      <c r="K74" t="inlineStr">
         <is>
           <t>42.28</t>
         </is>
@@ -4015,23 +4385,28 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
           <t>Torepe-Ormsby, aiko JR</t>
         </is>
       </c>
-      <c r="G75" t="n">
+      <c r="H75" t="n">
         <v>2</v>
       </c>
-      <c r="H75" t="inlineStr">
+      <c r="I75" t="inlineStr">
         <is>
           <t>19.45</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="J75" t="inlineStr">
         <is>
           <t>41.80</t>
         </is>
       </c>
-      <c r="J75" t="inlineStr">
+      <c r="K75" t="inlineStr">
         <is>
           <t>1:24.08</t>
         </is>
@@ -4063,23 +4438,28 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
           <t>Wiegand, Ben SR</t>
         </is>
       </c>
-      <c r="G76" t="n">
+      <c r="H76" t="n">
         <v>3</v>
       </c>
-      <c r="H76" t="inlineStr">
+      <c r="I76" t="inlineStr">
         <is>
           <t>19.49</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr">
+      <c r="J76" t="inlineStr">
         <is>
           <t>42.11</t>
         </is>
       </c>
-      <c r="J76" t="inlineStr">
+      <c r="K76" t="inlineStr">
         <is>
           <t>2:06.19</t>
         </is>
@@ -4111,23 +4491,28 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
           <t>Vainio, Luukas SO</t>
         </is>
       </c>
-      <c r="G77" t="n">
+      <c r="H77" t="n">
         <v>4</v>
       </c>
-      <c r="H77" t="inlineStr">
+      <c r="I77" t="inlineStr">
         <is>
           <t>20.50</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr">
+      <c r="J77" t="inlineStr">
         <is>
           <t>43.01</t>
         </is>
       </c>
-      <c r="J77" t="inlineStr">
+      <c r="K77" t="inlineStr">
         <is>
           <t>2:49.20</t>
         </is>
@@ -4159,23 +4544,28 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
           <t>Tirheimer, Logan 5Y</t>
         </is>
       </c>
-      <c r="G78" t="n">
-        <v>1</v>
-      </c>
-      <c r="H78" t="inlineStr">
+      <c r="H78" t="n">
+        <v>1</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>20.19</t>
         </is>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="J78" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
       </c>
-      <c r="J78" t="inlineStr">
+      <c r="K78" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
@@ -4207,23 +4597,28 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
           <t>Stoffle, Nate SR</t>
         </is>
       </c>
-      <c r="G79" t="n">
+      <c r="H79" t="n">
         <v>2</v>
       </c>
-      <c r="H79" t="inlineStr">
+      <c r="I79" t="inlineStr">
         <is>
           <t>19.99</t>
         </is>
       </c>
-      <c r="I79" t="inlineStr">
+      <c r="J79" t="inlineStr">
         <is>
           <t>42.50</t>
         </is>
       </c>
-      <c r="J79" t="inlineStr">
+      <c r="K79" t="inlineStr">
         <is>
           <t>1:24.90</t>
         </is>
@@ -4255,23 +4650,28 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
           <t>Husband, Ryan 5Y</t>
         </is>
       </c>
-      <c r="G80" t="n">
+      <c r="H80" t="n">
         <v>3</v>
       </c>
-      <c r="H80" t="inlineStr">
+      <c r="I80" t="inlineStr">
         <is>
           <t>19.89</t>
         </is>
       </c>
-      <c r="I80" t="inlineStr">
+      <c r="J80" t="inlineStr">
         <is>
           <t>42.14</t>
         </is>
       </c>
-      <c r="J80" t="inlineStr">
+      <c r="K80" t="inlineStr">
         <is>
           <t>2:07.04</t>
         </is>
@@ -4303,23 +4703,28 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
           <t>Schmidt, Danny JR</t>
         </is>
       </c>
-      <c r="G81" t="n">
+      <c r="H81" t="n">
         <v>4</v>
       </c>
-      <c r="H81" t="inlineStr">
+      <c r="I81" t="inlineStr">
         <is>
           <t>20.18</t>
         </is>
       </c>
-      <c r="I81" t="inlineStr">
+      <c r="J81" t="inlineStr">
         <is>
           <t>42.35</t>
         </is>
       </c>
-      <c r="J81" t="inlineStr">
+      <c r="K81" t="inlineStr">
         <is>
           <t>2:49.39</t>
         </is>
@@ -4351,23 +4756,28 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
+          <t>UNC</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
           <t>Hussey, Patrick 5Y</t>
         </is>
       </c>
-      <c r="G82" t="n">
-        <v>1</v>
-      </c>
-      <c r="H82" t="inlineStr">
+      <c r="H82" t="n">
+        <v>1</v>
+      </c>
+      <c r="I82" t="inlineStr">
         <is>
           <t>20.20</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr">
+      <c r="J82" t="inlineStr">
         <is>
           <t>42.13</t>
         </is>
       </c>
-      <c r="J82" t="inlineStr">
+      <c r="K82" t="inlineStr">
         <is>
           <t>42.13</t>
         </is>
@@ -4399,23 +4809,28 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
+          <t>UNC</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
           <t>Dramm, Louis JR</t>
         </is>
       </c>
-      <c r="G83" t="n">
+      <c r="H83" t="n">
         <v>2</v>
       </c>
-      <c r="H83" t="inlineStr">
+      <c r="I83" t="inlineStr">
         <is>
           <t>20.12</t>
         </is>
       </c>
-      <c r="I83" t="inlineStr">
+      <c r="J83" t="inlineStr">
         <is>
           <t>42.49</t>
         </is>
       </c>
-      <c r="J83" t="inlineStr">
+      <c r="K83" t="inlineStr">
         <is>
           <t>1:24.62</t>
         </is>
@@ -4447,23 +4862,28 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
+          <t>UNC</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
           <t>Foy, Patrick FR</t>
         </is>
       </c>
-      <c r="G84" t="n">
+      <c r="H84" t="n">
         <v>3</v>
       </c>
-      <c r="H84" t="inlineStr">
+      <c r="I84" t="inlineStr">
         <is>
           <t>19.86</t>
         </is>
       </c>
-      <c r="I84" t="inlineStr">
+      <c r="J84" t="inlineStr">
         <is>
           <t>42.61</t>
         </is>
       </c>
-      <c r="J84" t="inlineStr">
+      <c r="K84" t="inlineStr">
         <is>
           <t>2:07.23</t>
         </is>
@@ -4495,23 +4915,28 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
+          <t>UNC</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
           <t>Kartavi, Martin FR</t>
         </is>
       </c>
-      <c r="G85" t="n">
+      <c r="H85" t="n">
         <v>4</v>
       </c>
-      <c r="H85" t="inlineStr">
+      <c r="I85" t="inlineStr">
         <is>
           <t>19.68</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr">
+      <c r="J85" t="inlineStr">
         <is>
           <t>42.21</t>
         </is>
       </c>
-      <c r="J85" t="inlineStr">
+      <c r="K85" t="inlineStr">
         <is>
           <t>2:49.44</t>
         </is>
@@ -4543,23 +4968,28 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
+          <t>LSU</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
           <t>Hribar, Jere SO</t>
         </is>
       </c>
-      <c r="G86" t="n">
-        <v>1</v>
-      </c>
-      <c r="H86" t="inlineStr">
+      <c r="H86" t="n">
+        <v>1</v>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>19.84</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr">
+      <c r="J86" t="inlineStr">
         <is>
           <t>41.55</t>
         </is>
       </c>
-      <c r="J86" t="inlineStr">
+      <c r="K86" t="inlineStr">
         <is>
           <t>41.55</t>
         </is>
@@ -4591,23 +5021,28 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
+          <t>LSU</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
           <t>Goncharov, Stepan JR</t>
         </is>
       </c>
-      <c r="G87" t="n">
+      <c r="H87" t="n">
         <v>2</v>
       </c>
-      <c r="H87" t="inlineStr">
+      <c r="I87" t="inlineStr">
         <is>
           <t>19.72</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr">
+      <c r="J87" t="inlineStr">
         <is>
           <t>42.27</t>
         </is>
       </c>
-      <c r="J87" t="inlineStr">
+      <c r="K87" t="inlineStr">
         <is>
           <t>1:23.82</t>
         </is>
@@ -4639,23 +5074,28 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
+          <t>LSU</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
           <t>Garon, Andrew JR</t>
         </is>
       </c>
-      <c r="G88" t="n">
+      <c r="H88" t="n">
         <v>3</v>
       </c>
-      <c r="H88" t="inlineStr">
+      <c r="I88" t="inlineStr">
         <is>
           <t>20.35</t>
         </is>
       </c>
-      <c r="I88" t="inlineStr">
+      <c r="J88" t="inlineStr">
         <is>
           <t>42.87</t>
         </is>
       </c>
-      <c r="J88" t="inlineStr">
+      <c r="K88" t="inlineStr">
         <is>
           <t>2:06.69</t>
         </is>
@@ -4687,23 +5127,28 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
+          <t>LSU</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
           <t>Curtis, Griffin SR</t>
         </is>
       </c>
-      <c r="G89" t="n">
+      <c r="H89" t="n">
         <v>4</v>
       </c>
-      <c r="H89" t="inlineStr">
+      <c r="I89" t="inlineStr">
         <is>
           <t>20.16</t>
         </is>
       </c>
-      <c r="I89" t="inlineStr">
+      <c r="J89" t="inlineStr">
         <is>
           <t>42.77</t>
         </is>
       </c>
-      <c r="J89" t="inlineStr">
+      <c r="K89" t="inlineStr">
         <is>
           <t>2:49.46</t>
         </is>
@@ -4735,23 +5180,28 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
+          <t>Yale</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
           <t>Finch, Nicholas FR</t>
         </is>
       </c>
-      <c r="G90" t="n">
-        <v>1</v>
-      </c>
-      <c r="H90" t="inlineStr">
+      <c r="H90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>20.51</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr">
+      <c r="J90" t="inlineStr">
         <is>
           <t>43.03</t>
         </is>
       </c>
-      <c r="J90" t="inlineStr">
+      <c r="K90" t="inlineStr">
         <is>
           <t>43.03</t>
         </is>
@@ -4783,23 +5233,28 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
+          <t>Yale</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
           <t>Nankov, Deniel SO</t>
         </is>
       </c>
-      <c r="G91" t="n">
+      <c r="H91" t="n">
         <v>2</v>
       </c>
-      <c r="H91" t="inlineStr">
+      <c r="I91" t="inlineStr">
         <is>
           <t>19.72</t>
         </is>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="J91" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
       </c>
-      <c r="J91" t="inlineStr">
+      <c r="K91" t="inlineStr">
         <is>
           <t>1:25.43</t>
         </is>
@@ -4831,23 +5286,28 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
+          <t>Yale</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
           <t>Wang, Jake FR</t>
         </is>
       </c>
-      <c r="G92" t="n">
+      <c r="H92" t="n">
         <v>3</v>
       </c>
-      <c r="H92" t="inlineStr">
+      <c r="I92" t="inlineStr">
         <is>
           <t>19.58</t>
         </is>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="J92" t="inlineStr">
         <is>
           <t>42.07</t>
         </is>
       </c>
-      <c r="J92" t="inlineStr">
+      <c r="K92" t="inlineStr">
         <is>
           <t>2:07.50</t>
         </is>
@@ -4879,23 +5339,28 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
+          <t>Yale</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
           <t>Millard, Noah JR</t>
         </is>
       </c>
-      <c r="G93" t="n">
+      <c r="H93" t="n">
         <v>4</v>
       </c>
-      <c r="H93" t="inlineStr">
+      <c r="I93" t="inlineStr">
         <is>
           <t>20.16</t>
         </is>
       </c>
-      <c r="I93" t="inlineStr">
+      <c r="J93" t="inlineStr">
         <is>
           <t>42.64</t>
         </is>
       </c>
-      <c r="J93" t="inlineStr">
+      <c r="K93" t="inlineStr">
         <is>
           <t>2:50.14</t>
         </is>
@@ -4927,23 +5392,28 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
+          <t>Northwestern</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
           <t>Seymour, Stuart SO</t>
         </is>
       </c>
-      <c r="G94" t="n">
-        <v>1</v>
-      </c>
-      <c r="H94" t="inlineStr">
+      <c r="H94" t="n">
+        <v>1</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>20.42</t>
         </is>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="J94" t="inlineStr">
         <is>
           <t>42.73</t>
         </is>
       </c>
-      <c r="J94" t="inlineStr">
+      <c r="K94" t="inlineStr">
         <is>
           <t>42.73</t>
         </is>
@@ -4975,23 +5445,28 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
+          <t>Northwestern</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
           <t>Duncan, Cade SO</t>
         </is>
       </c>
-      <c r="G95" t="n">
+      <c r="H95" t="n">
         <v>2</v>
       </c>
-      <c r="H95" t="inlineStr">
+      <c r="I95" t="inlineStr">
         <is>
           <t>19.94</t>
         </is>
       </c>
-      <c r="I95" t="inlineStr">
+      <c r="J95" t="inlineStr">
         <is>
           <t>41.88</t>
         </is>
       </c>
-      <c r="J95" t="inlineStr">
+      <c r="K95" t="inlineStr">
         <is>
           <t>1:24.61</t>
         </is>
@@ -5023,23 +5498,28 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
+          <t>Northwestern</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
           <t>Schuster, Connor SO</t>
         </is>
       </c>
-      <c r="G96" t="n">
+      <c r="H96" t="n">
         <v>3</v>
       </c>
-      <c r="H96" t="inlineStr">
+      <c r="I96" t="inlineStr">
         <is>
           <t>19.91</t>
         </is>
       </c>
-      <c r="I96" t="inlineStr">
+      <c r="J96" t="inlineStr">
         <is>
           <t>42.79</t>
         </is>
       </c>
-      <c r="J96" t="inlineStr">
+      <c r="K96" t="inlineStr">
         <is>
           <t>2:07.40</t>
         </is>
@@ -5071,23 +5551,28 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
+          <t>Northwestern</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
           <t>Gerchik, David SO</t>
         </is>
       </c>
-      <c r="G97" t="n">
+      <c r="H97" t="n">
         <v>4</v>
       </c>
-      <c r="H97" t="inlineStr">
+      <c r="I97" t="inlineStr">
         <is>
           <t>20.06</t>
         </is>
       </c>
-      <c r="I97" t="inlineStr">
+      <c r="J97" t="inlineStr">
         <is>
           <t>42.91</t>
         </is>
       </c>
-      <c r="J97" t="inlineStr">
+      <c r="K97" t="inlineStr">
         <is>
           <t>2:50.31</t>
         </is>
@@ -5119,23 +5604,28 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
+          <t>USC</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
           <t>Sogaard-Andersen, Oliver FR</t>
         </is>
       </c>
-      <c r="G98" t="n">
-        <v>1</v>
-      </c>
-      <c r="H98" t="inlineStr">
+      <c r="H98" t="n">
+        <v>1</v>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>20.18</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr">
+      <c r="J98" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
       </c>
-      <c r="J98" t="inlineStr">
+      <c r="K98" t="inlineStr">
         <is>
           <t>42.40</t>
         </is>
@@ -5167,23 +5657,28 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
+          <t>USC</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
           <t>Maurer, Luke 5Y</t>
         </is>
       </c>
-      <c r="G99" t="n">
+      <c r="H99" t="n">
         <v>2</v>
       </c>
-      <c r="H99" t="inlineStr">
+      <c r="I99" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="I99" t="inlineStr">
+      <c r="J99" t="inlineStr">
         <is>
           <t>42.22</t>
         </is>
       </c>
-      <c r="J99" t="inlineStr">
+      <c r="K99" t="inlineStr">
         <is>
           <t>1:24.62</t>
         </is>
@@ -5215,23 +5710,28 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
+          <t>USC</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
           <t>Chmielewski, Krztof SO</t>
         </is>
       </c>
-      <c r="G100" t="n">
+      <c r="H100" t="n">
         <v>3</v>
       </c>
-      <c r="H100" t="inlineStr">
+      <c r="I100" t="inlineStr">
         <is>
           <t>20.43</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr">
+      <c r="J100" t="inlineStr">
         <is>
           <t>43.11</t>
         </is>
       </c>
-      <c r="J100" t="inlineStr">
+      <c r="K100" t="inlineStr">
         <is>
           <t>2:07.73</t>
         </is>
@@ -5263,23 +5763,28 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
+          <t>USC</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
           <t>Dillingham, Diggory FR</t>
         </is>
       </c>
-      <c r="G101" t="n">
+      <c r="H101" t="n">
         <v>4</v>
       </c>
-      <c r="H101" t="inlineStr">
+      <c r="I101" t="inlineStr">
         <is>
           <t>19.97</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr">
+      <c r="J101" t="inlineStr">
         <is>
           <t>42.75</t>
         </is>
       </c>
-      <c r="J101" t="inlineStr">
+      <c r="K101" t="inlineStr">
         <is>
           <t>2:50.48</t>
         </is>
@@ -5311,23 +5816,28 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
+          <t>SMU</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
           <t>Lockhart, Wade SR</t>
         </is>
       </c>
-      <c r="G102" t="n">
-        <v>1</v>
-      </c>
-      <c r="H102" t="inlineStr">
+      <c r="H102" t="n">
+        <v>1</v>
+      </c>
+      <c r="I102" t="inlineStr">
         <is>
           <t>20.33</t>
         </is>
       </c>
-      <c r="I102" t="inlineStr">
+      <c r="J102" t="inlineStr">
         <is>
           <t>42.62</t>
         </is>
       </c>
-      <c r="J102" t="inlineStr">
+      <c r="K102" t="inlineStr">
         <is>
           <t>42.62</t>
         </is>
@@ -5359,23 +5869,28 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
+          <t>SMU</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
           <t>Sungail, Sage JR</t>
         </is>
       </c>
-      <c r="G103" t="n">
+      <c r="H103" t="n">
         <v>2</v>
       </c>
-      <c r="H103" t="inlineStr">
+      <c r="I103" t="inlineStr">
         <is>
           <t>20.17</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr">
+      <c r="J103" t="inlineStr">
         <is>
           <t>42.47</t>
         </is>
       </c>
-      <c r="J103" t="inlineStr">
+      <c r="K103" t="inlineStr">
         <is>
           <t>1:25.09</t>
         </is>
@@ -5407,23 +5922,28 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
+          <t>SMU</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
           <t>Butler, Lance 5Y</t>
         </is>
       </c>
-      <c r="G104" t="n">
+      <c r="H104" t="n">
         <v>3</v>
       </c>
-      <c r="H104" t="inlineStr">
+      <c r="I104" t="inlineStr">
         <is>
           <t>19.88</t>
         </is>
       </c>
-      <c r="I104" t="inlineStr">
+      <c r="J104" t="inlineStr">
         <is>
           <t>42.39</t>
         </is>
       </c>
-      <c r="J104" t="inlineStr">
+      <c r="K104" t="inlineStr">
         <is>
           <t>2:07.48</t>
         </is>
@@ -5455,23 +5975,28 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
+          <t>SMU</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
           <t>Forrest, Jack JR</t>
         </is>
       </c>
-      <c r="G105" t="n">
+      <c r="H105" t="n">
         <v>4</v>
       </c>
-      <c r="H105" t="inlineStr">
+      <c r="I105" t="inlineStr">
         <is>
           <t>20.71</t>
         </is>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="J105" t="inlineStr">
         <is>
           <t>43.63</t>
         </is>
       </c>
-      <c r="J105" t="inlineStr">
+      <c r="K105" t="inlineStr">
         <is>
           <t>2:51.11</t>
         </is>
@@ -5503,23 +6028,28 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
+          <t>Princeton</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
           <t>Dinu, Patrick FR</t>
         </is>
       </c>
-      <c r="G106" t="n">
-        <v>1</v>
-      </c>
-      <c r="H106" t="inlineStr">
+      <c r="H106" t="n">
+        <v>1</v>
+      </c>
+      <c r="I106" t="inlineStr">
         <is>
           <t>20.15</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr">
+      <c r="J106" t="inlineStr">
         <is>
           <t>42.15</t>
         </is>
       </c>
-      <c r="J106" t="inlineStr">
+      <c r="K106" t="inlineStr">
         <is>
           <t>42.15</t>
         </is>
@@ -5551,23 +6081,28 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
+          <t>Princeton</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
           <t>Schott, Mitchell JR</t>
         </is>
       </c>
-      <c r="G107" t="n">
+      <c r="H107" t="n">
         <v>2</v>
       </c>
-      <c r="H107" t="inlineStr">
+      <c r="I107" t="inlineStr">
         <is>
           <t>20.11</t>
         </is>
       </c>
-      <c r="I107" t="inlineStr">
+      <c r="J107" t="inlineStr">
         <is>
           <t>42.17</t>
         </is>
       </c>
-      <c r="J107" t="inlineStr">
+      <c r="K107" t="inlineStr">
         <is>
           <t>1:24.32</t>
         </is>
@@ -5599,23 +6134,28 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
+          <t>Princeton</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
           <t>Sech, Noah SO</t>
         </is>
       </c>
-      <c r="G108" t="n">
+      <c r="H108" t="n">
         <v>3</v>
       </c>
-      <c r="H108" t="inlineStr">
+      <c r="I108" t="inlineStr">
         <is>
           <t>20.62</t>
         </is>
       </c>
-      <c r="I108" t="inlineStr">
+      <c r="J108" t="inlineStr">
         <is>
           <t>44.00</t>
         </is>
       </c>
-      <c r="J108" t="inlineStr">
+      <c r="K108" t="inlineStr">
         <is>
           <t>2:08.32</t>
         </is>
@@ -5647,23 +6187,28 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
+          <t>Princeton</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
           <t>Feyerick, Brett SR</t>
         </is>
       </c>
-      <c r="G109" t="n">
+      <c r="H109" t="n">
         <v>4</v>
       </c>
-      <c r="H109" t="inlineStr">
+      <c r="I109" t="inlineStr">
         <is>
           <t>20.01</t>
         </is>
       </c>
-      <c r="I109" t="inlineStr">
+      <c r="J109" t="inlineStr">
         <is>
           <t>43.08</t>
         </is>
       </c>
-      <c r="J109" t="inlineStr">
+      <c r="K109" t="inlineStr">
         <is>
           <t>2:51.40</t>
         </is>
@@ -5695,23 +6240,28 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
           <t>Odorici, Leandro SR</t>
         </is>
       </c>
-      <c r="G110" t="n">
-        <v>1</v>
-      </c>
-      <c r="H110" t="inlineStr">
+      <c r="H110" t="n">
+        <v>1</v>
+      </c>
+      <c r="I110" t="inlineStr">
         <is>
           <t>20.42</t>
         </is>
       </c>
-      <c r="I110" t="inlineStr">
+      <c r="J110" t="inlineStr">
         <is>
           <t>43.05</t>
         </is>
       </c>
-      <c r="J110" t="inlineStr">
+      <c r="K110" t="inlineStr">
         <is>
           <t>43.05</t>
         </is>
@@ -5743,23 +6293,28 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
           <t>Saka, Berke SR</t>
         </is>
       </c>
-      <c r="G111" t="n">
+      <c r="H111" t="n">
         <v>2</v>
       </c>
-      <c r="H111" t="inlineStr">
+      <c r="I111" t="inlineStr">
         <is>
           <t>19.85</t>
         </is>
       </c>
-      <c r="I111" t="inlineStr">
+      <c r="J111" t="inlineStr">
         <is>
           <t>42.63</t>
         </is>
       </c>
-      <c r="J111" t="inlineStr">
+      <c r="K111" t="inlineStr">
         <is>
           <t>1:25.68</t>
         </is>
@@ -5791,23 +6346,28 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
           <t>Yeboah, Robin SO</t>
         </is>
       </c>
-      <c r="G112" t="n">
+      <c r="H112" t="n">
         <v>3</v>
       </c>
-      <c r="H112" t="inlineStr">
+      <c r="I112" t="inlineStr">
         <is>
           <t>19.90</t>
         </is>
       </c>
-      <c r="I112" t="inlineStr">
+      <c r="J112" t="inlineStr">
         <is>
           <t>42.70</t>
         </is>
       </c>
-      <c r="J112" t="inlineStr">
+      <c r="K112" t="inlineStr">
         <is>
           <t>2:08.38</t>
         </is>
@@ -5839,23 +6399,28 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
           <t>Gapinski, David SR</t>
         </is>
       </c>
-      <c r="G113" t="n">
+      <c r="H113" t="n">
         <v>4</v>
       </c>
-      <c r="H113" t="inlineStr">
+      <c r="I113" t="inlineStr">
         <is>
           <t>20.04</t>
         </is>
       </c>
-      <c r="I113" t="inlineStr">
+      <c r="J113" t="inlineStr">
         <is>
           <t>43.30</t>
         </is>
       </c>
-      <c r="J113" t="inlineStr">
+      <c r="K113" t="inlineStr">
         <is>
           <t>2:51.68</t>
         </is>
@@ -5887,23 +6452,28 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
           <t>Bochenski, Grant SR</t>
         </is>
       </c>
-      <c r="G114" t="n">
-        <v>1</v>
-      </c>
-      <c r="H114" t="inlineStr">
+      <c r="H114" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" t="inlineStr">
         <is>
           <t>20.19</t>
         </is>
       </c>
-      <c r="I114" t="inlineStr">
+      <c r="J114" t="inlineStr">
         <is>
           <t>42.59</t>
         </is>
       </c>
-      <c r="J114" t="inlineStr">
+      <c r="K114" t="inlineStr">
         <is>
           <t>42.59</t>
         </is>
@@ -5935,23 +6505,28 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
           <t>Nebrich, Lucas FR</t>
         </is>
       </c>
-      <c r="G115" t="n">
+      <c r="H115" t="n">
         <v>2</v>
       </c>
-      <c r="H115" t="inlineStr">
+      <c r="I115" t="inlineStr">
         <is>
           <t>19.81</t>
         </is>
       </c>
-      <c r="I115" t="inlineStr">
+      <c r="J115" t="inlineStr">
         <is>
           <t>42.76</t>
         </is>
       </c>
-      <c r="J115" t="inlineStr">
+      <c r="K115" t="inlineStr">
         <is>
           <t>1:25.35</t>
         </is>
@@ -5983,23 +6558,28 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
           <t>Vance, Ethan FR</t>
         </is>
       </c>
-      <c r="G116" t="n">
+      <c r="H116" t="n">
         <v>3</v>
       </c>
-      <c r="H116" t="inlineStr">
+      <c r="I116" t="inlineStr">
         <is>
           <t>20.22</t>
         </is>
       </c>
-      <c r="I116" t="inlineStr">
+      <c r="J116" t="inlineStr">
         <is>
           <t>43.03</t>
         </is>
       </c>
-      <c r="J116" t="inlineStr">
+      <c r="K116" t="inlineStr">
         <is>
           <t>2:08.38</t>
         </is>
@@ -6031,23 +6611,28 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
           <t>Tate, Darden SO</t>
         </is>
       </c>
-      <c r="G117" t="n">
+      <c r="H117" t="n">
         <v>4</v>
       </c>
-      <c r="H117" t="inlineStr">
+      <c r="I117" t="inlineStr">
         <is>
           <t>20.51</t>
         </is>
       </c>
-      <c r="I117" t="inlineStr">
+      <c r="J117" t="inlineStr">
         <is>
           <t>43.84</t>
         </is>
       </c>
-      <c r="J117" t="inlineStr">
+      <c r="K117" t="inlineStr">
         <is>
           <t>2:52.22</t>
         </is>
@@ -6079,23 +6664,28 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
+          <t>Harvard</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
           <t>Wang, Sonny SO</t>
         </is>
       </c>
-      <c r="G118" t="n">
-        <v>1</v>
-      </c>
-      <c r="H118" t="inlineStr">
+      <c r="H118" t="n">
+        <v>1</v>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>20.44</t>
         </is>
       </c>
-      <c r="I118" t="inlineStr">
+      <c r="J118" t="inlineStr">
         <is>
           <t>43.02</t>
         </is>
       </c>
-      <c r="J118" t="inlineStr">
+      <c r="K118" t="inlineStr">
         <is>
           <t>43.02</t>
         </is>
@@ -6127,23 +6717,28 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
+          <t>Harvard</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
           <t>Greeley, David JR</t>
         </is>
       </c>
-      <c r="G119" t="n">
+      <c r="H119" t="n">
         <v>2</v>
       </c>
-      <c r="H119" t="inlineStr">
+      <c r="I119" t="inlineStr">
         <is>
           <t>20.13</t>
         </is>
       </c>
-      <c r="I119" t="inlineStr">
+      <c r="J119" t="inlineStr">
         <is>
           <t>43.07</t>
         </is>
       </c>
-      <c r="J119" t="inlineStr">
+      <c r="K119" t="inlineStr">
         <is>
           <t>1:26.09</t>
         </is>
@@ -6175,23 +6770,28 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
+          <t>Harvard</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
           <t>Gattnar, Marre FR</t>
         </is>
       </c>
-      <c r="G120" t="n">
+      <c r="H120" t="n">
         <v>3</v>
       </c>
-      <c r="H120" t="inlineStr">
+      <c r="I120" t="inlineStr">
         <is>
           <t>20.05</t>
         </is>
       </c>
-      <c r="I120" t="inlineStr">
+      <c r="J120" t="inlineStr">
         <is>
           <t>43.03</t>
         </is>
       </c>
-      <c r="J120" t="inlineStr">
+      <c r="K120" t="inlineStr">
         <is>
           <t>2:09.12</t>
         </is>
@@ -6223,23 +6823,28 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
+          <t>Harvard</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
           <t>Croley, Evan FR</t>
         </is>
       </c>
-      <c r="G121" t="n">
+      <c r="H121" t="n">
         <v>4</v>
       </c>
-      <c r="H121" t="inlineStr">
+      <c r="I121" t="inlineStr">
         <is>
           <t>20.14</t>
         </is>
       </c>
-      <c r="I121" t="inlineStr">
+      <c r="J121" t="inlineStr">
         <is>
           <t>43.24</t>
         </is>
       </c>
-      <c r="J121" t="inlineStr">
+      <c r="K121" t="inlineStr">
         <is>
           <t>2:52.36</t>
         </is>

</xml_diff>